<commit_message>
Fix cartesian type in CSProjection
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1475,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1936,7 +1936,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>328</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:2">

</xml_diff>

<commit_message>
Add Heightmap structure object
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1475,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1992,7 +1992,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2526,7 +2526,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
     </row>
     <row r="134" spans="1:2">

</xml_diff>

<commit_message>
More Ellipsoid terrain work, add CSTerrainMesh
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1475,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2526,7 +2526,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>328</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2534,7 +2534,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="135" spans="1:2">

</xml_diff>

<commit_message>
Update status worksheet with swift port status
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="540" windowWidth="18520" windowHeight="24240" tabRatio="500"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="29060" windowHeight="18580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="339">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1030,6 +1030,12 @@
   </si>
   <si>
     <t>interface only</t>
+  </si>
+  <si>
+    <t>Swift port</t>
+  </si>
+  <si>
+    <t>Missing array return bug</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1048,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1088,7 +1093,235 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1473,25 +1706,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C331"/>
+  <dimension ref="A1:D331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="48" customWidth="1"/>
+    <col min="2" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1">
+    <row r="3" spans="1:4" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1499,695 +1732,950 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1">
+    <row r="5" spans="1:4" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>328</v>
+      </c>
+      <c r="D52" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B71" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="C80" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="C82" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="C83" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="C84" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="C85" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="C86" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="C87" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="C88" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="C89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="C90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="C91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
@@ -2195,170 +2683,233 @@
         <v>328</v>
       </c>
       <c r="C92" t="s">
+        <v>191</v>
+      </c>
+      <c r="D92" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="C93" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="C94" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="C95" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B107" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B108" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B109" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B110" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B111" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="C112" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
         <v>111</v>
       </c>
@@ -2366,362 +2917,497 @@
         <v>328</v>
       </c>
       <c r="C113" t="s">
+        <v>191</v>
+      </c>
+      <c r="D113" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B114" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="C114" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B115" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="C115" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B116" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="C116" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B117" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="C117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B118" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="C118" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B119" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="C119" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B120" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="C120" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B121" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="C121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B122" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="C122" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="C123" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B124" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="C124" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B125" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="C125" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B126" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="C126" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B127" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="C127" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B128" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="C128" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B129" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="C129" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B130" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="C130" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B131" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="C131" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B132" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="C132" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B133" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="C133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B134" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="C134" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B135" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="C135" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B136" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="C136" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B137" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="C137" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B138" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="C138" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B139" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="C139" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
       <c r="A140" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B140" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="C140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B141" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="C141" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B142" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="C142" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B143" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="C143" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
       <c r="A144" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B144" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="C144" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B145" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="C145" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B146" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="C146" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B147" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="C147" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B148" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="C148" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B149" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="C149" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B150" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="C150" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B151" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="C151" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B152" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="C152" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B153" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="C153" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B154" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="C154" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B155" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="156" spans="1:3">
+      <c r="C155" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B156" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="157" spans="1:3">
+      <c r="C156" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B157" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="C157" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="2" t="s">
         <v>156</v>
       </c>
@@ -2729,10 +3415,13 @@
         <v>190</v>
       </c>
       <c r="C158" t="s">
+        <v>191</v>
+      </c>
+      <c r="D158" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:4">
       <c r="A159" s="2" t="s">
         <v>157</v>
       </c>
@@ -2740,10 +3429,13 @@
         <v>190</v>
       </c>
       <c r="C159" t="s">
+        <v>191</v>
+      </c>
+      <c r="D159" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:4">
       <c r="A160" s="2" t="s">
         <v>158</v>
       </c>
@@ -2751,58 +3443,79 @@
         <v>190</v>
       </c>
       <c r="C160" t="s">
+        <v>191</v>
+      </c>
+      <c r="D160" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:4">
       <c r="A161" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B161" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="C161" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B162" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="C162" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B163" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="C163" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B164" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="C164" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B165" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="C165" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B166" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="C166" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="2" t="s">
         <v>165</v>
       </c>
@@ -2810,263 +3523,359 @@
         <v>190</v>
       </c>
       <c r="C167" t="s">
+        <v>191</v>
+      </c>
+      <c r="D167" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:4">
       <c r="A168" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B168" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="169" spans="1:3">
+      <c r="C168" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B169" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="170" spans="1:3">
+      <c r="C169" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B170" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="171" spans="1:3">
+      <c r="C170" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B171" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="172" spans="1:3">
+      <c r="C171" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B172" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="C172" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B173" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="C173" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B174" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="C174" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B175" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="C175" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B176" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="177" spans="1:2">
+      <c r="C176" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B177" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="178" spans="1:2">
+      <c r="C177" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B178" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="179" spans="1:2">
+      <c r="C178" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B179" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="180" spans="1:2">
+      <c r="C179" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B180" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="181" spans="1:2">
+      <c r="C180" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B181" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="182" spans="1:2">
+      <c r="C181" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B182" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="183" spans="1:2">
+      <c r="C182" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B183" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="184" spans="1:2">
+      <c r="C183" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
       <c r="A184" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B184" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="185" spans="1:2">
+      <c r="C184" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B185" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="186" spans="1:2">
+      <c r="C185" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B186" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="187" spans="1:2">
+      <c r="C186" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B187" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="188" spans="1:2">
+      <c r="C187" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B188" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="189" spans="1:2">
+      <c r="C188" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
       <c r="A189" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B189" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="190" spans="1:2">
+      <c r="C189" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B190" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="191" spans="1:2">
+      <c r="C190" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B191" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:3">
+      <c r="C191" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
       <c r="A193" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>194</v>
       </c>
       <c r="B195" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="196" spans="1:3">
+      <c r="C195" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>195</v>
       </c>
       <c r="B196" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="197" spans="1:3">
+      <c r="C196" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>196</v>
       </c>
       <c r="B197" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="198" spans="1:3">
+      <c r="C197" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>197</v>
       </c>
       <c r="B198" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="199" spans="1:3">
+      <c r="C198" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>198</v>
       </c>
       <c r="B199" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="200" spans="1:3">
+      <c r="C199" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>199</v>
       </c>
       <c r="B200" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="201" spans="1:3">
+      <c r="C200" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>200</v>
       </c>
       <c r="B201" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="202" spans="1:3">
+      <c r="C201" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3074,26 +3883,35 @@
         <v>328</v>
       </c>
       <c r="C202" t="s">
+        <v>191</v>
+      </c>
+      <c r="D202" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>202</v>
       </c>
       <c r="B203" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="204" spans="1:3">
+      <c r="C203" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>203</v>
       </c>
       <c r="B204" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="205" spans="1:3">
+      <c r="C204" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3101,26 +3919,35 @@
         <v>328</v>
       </c>
       <c r="C205" t="s">
+        <v>191</v>
+      </c>
+      <c r="D205" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>205</v>
       </c>
       <c r="B206" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="207" spans="1:3">
+      <c r="C206" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>206</v>
       </c>
       <c r="B207" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="208" spans="1:3">
+      <c r="C207" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3128,82 +3955,112 @@
         <v>328</v>
       </c>
       <c r="C208" t="s">
+        <v>191</v>
+      </c>
+      <c r="D208" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>208</v>
       </c>
       <c r="B209" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="210" spans="1:3">
+      <c r="C209" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>209</v>
       </c>
       <c r="B210" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="211" spans="1:3">
+      <c r="C210" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>210</v>
       </c>
       <c r="B211" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="212" spans="1:3">
+      <c r="C211" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>211</v>
       </c>
       <c r="B212" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="213" spans="1:3">
+      <c r="C212" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>212</v>
       </c>
       <c r="B213" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="214" spans="1:3">
+      <c r="C213" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>213</v>
       </c>
       <c r="B214" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="215" spans="1:3">
+      <c r="C214" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>214</v>
       </c>
       <c r="B215" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="216" spans="1:3">
+      <c r="C215" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
         <v>215</v>
       </c>
       <c r="B216" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="217" spans="1:3">
+      <c r="C216" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="218" spans="1:3">
+      <c r="C217" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3211,895 +4068,1222 @@
         <v>191</v>
       </c>
       <c r="C218" t="s">
+        <v>191</v>
+      </c>
+      <c r="D218" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>218</v>
       </c>
       <c r="B219" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="220" spans="1:3">
+      <c r="C219" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>219</v>
       </c>
       <c r="B220" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="221" spans="1:3">
+      <c r="C220" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>220</v>
       </c>
       <c r="B221" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="222" spans="1:3">
+      <c r="C221" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>221</v>
       </c>
       <c r="B222" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="224" spans="1:3">
+      <c r="C222" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:3">
       <c r="A226" t="s">
         <v>223</v>
       </c>
       <c r="B226" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="227" spans="1:2">
+      <c r="C226" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
       <c r="A227" t="s">
         <v>224</v>
       </c>
       <c r="B227" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="228" spans="1:2">
+      <c r="C227" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
       <c r="A228" t="s">
         <v>225</v>
       </c>
       <c r="B228" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="229" spans="1:2">
+      <c r="C228" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
       <c r="A229" t="s">
         <v>226</v>
       </c>
       <c r="B229" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="230" spans="1:2">
+      <c r="C229" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
       <c r="A230" t="s">
         <v>227</v>
       </c>
       <c r="B230" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="231" spans="1:2">
+      <c r="C230" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
       <c r="A231" t="s">
         <v>228</v>
       </c>
       <c r="B231" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="232" spans="1:2">
+      <c r="C231" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
       <c r="A232" t="s">
         <v>229</v>
       </c>
       <c r="B232" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="233" spans="1:2">
+      <c r="C232" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
       <c r="A233" t="s">
         <v>230</v>
       </c>
       <c r="B233" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="234" spans="1:2">
+      <c r="C233" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
       <c r="A234" t="s">
         <v>231</v>
       </c>
       <c r="B234" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="235" spans="1:2">
+      <c r="C234" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
       <c r="A235" t="s">
         <v>232</v>
       </c>
       <c r="B235" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="236" spans="1:2">
+      <c r="C235" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
       <c r="A236" t="s">
         <v>233</v>
       </c>
       <c r="B236" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="237" spans="1:2">
+      <c r="C236" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
       <c r="A237" t="s">
         <v>234</v>
       </c>
       <c r="B237" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="238" spans="1:2">
+      <c r="C237" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>235</v>
       </c>
       <c r="B238" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="239" spans="1:2">
+      <c r="C238" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
       <c r="A239" t="s">
         <v>236</v>
       </c>
       <c r="B239" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="240" spans="1:2">
+      <c r="C239" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
       <c r="A240" t="s">
         <v>237</v>
       </c>
       <c r="B240" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="241" spans="1:2">
+      <c r="C240" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>238</v>
       </c>
       <c r="B241" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="242" spans="1:2">
+      <c r="C241" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
       <c r="A242" t="s">
         <v>239</v>
       </c>
       <c r="B242" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="243" spans="1:2">
+      <c r="C242" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
       <c r="A243" t="s">
         <v>240</v>
       </c>
       <c r="B243" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="244" spans="1:2">
+      <c r="C243" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>241</v>
       </c>
       <c r="B244" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="245" spans="1:2">
+      <c r="C244" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
       <c r="A245" t="s">
         <v>242</v>
       </c>
       <c r="B245" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="246" spans="1:2">
+      <c r="C245" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
       <c r="A246" t="s">
         <v>243</v>
       </c>
       <c r="B246" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="247" spans="1:2">
+      <c r="C246" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
       <c r="A247" t="s">
         <v>244</v>
       </c>
       <c r="B247" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="248" spans="1:2">
+      <c r="C247" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
       <c r="A248" t="s">
         <v>245</v>
       </c>
       <c r="B248" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="249" spans="1:2">
+      <c r="C248" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
       <c r="A249" t="s">
         <v>246</v>
       </c>
       <c r="B249" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="250" spans="1:2">
+      <c r="C249" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
       <c r="A250" t="s">
         <v>247</v>
       </c>
       <c r="B250" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="251" spans="1:2">
+      <c r="C250" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
       <c r="A251" t="s">
         <v>248</v>
       </c>
       <c r="B251" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="252" spans="1:2">
+      <c r="C251" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
       <c r="A252" t="s">
         <v>249</v>
       </c>
       <c r="B252" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="253" spans="1:2">
+      <c r="C252" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
       <c r="A253" t="s">
         <v>250</v>
       </c>
       <c r="B253" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="254" spans="1:2">
+      <c r="C253" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
       <c r="A254" t="s">
         <v>251</v>
       </c>
       <c r="B254" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="255" spans="1:2">
+      <c r="C254" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
       <c r="A255" t="s">
         <v>252</v>
       </c>
       <c r="B255" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="256" spans="1:2">
+      <c r="C255" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
       <c r="A256" t="s">
         <v>253</v>
       </c>
       <c r="B256" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="257" spans="1:2">
+      <c r="C256" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>254</v>
       </c>
       <c r="B257" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="258" spans="1:2">
+      <c r="C257" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
       <c r="A258" t="s">
         <v>255</v>
       </c>
       <c r="B258" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="259" spans="1:2">
+      <c r="C258" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
       <c r="A259" t="s">
         <v>256</v>
       </c>
       <c r="B259" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="260" spans="1:2">
+      <c r="C259" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
       <c r="A260" t="s">
         <v>257</v>
       </c>
       <c r="B260" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="261" spans="1:2">
+      <c r="C260" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>258</v>
       </c>
       <c r="B261" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="262" spans="1:2">
+      <c r="C261" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>259</v>
       </c>
       <c r="B262" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="263" spans="1:2">
+      <c r="C262" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>260</v>
       </c>
       <c r="B263" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="264" spans="1:2">
+      <c r="C263" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
       <c r="A264" t="s">
         <v>261</v>
       </c>
       <c r="B264" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="265" spans="1:2">
+      <c r="C264" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
       <c r="A265" t="s">
         <v>262</v>
       </c>
       <c r="B265" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="266" spans="1:2">
+      <c r="C265" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
       <c r="A266" t="s">
         <v>263</v>
       </c>
       <c r="B266" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="267" spans="1:2">
+      <c r="C266" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
       <c r="A267" t="s">
         <v>264</v>
       </c>
       <c r="B267" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="268" spans="1:2">
+      <c r="C267" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>265</v>
       </c>
       <c r="B268" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="269" spans="1:2">
+      <c r="C268" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
       <c r="A269" t="s">
         <v>266</v>
       </c>
       <c r="B269" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="270" spans="1:2">
+      <c r="C269" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
       <c r="A270" t="s">
         <v>267</v>
       </c>
       <c r="B270" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="271" spans="1:2">
+      <c r="C270" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
       <c r="A271" t="s">
         <v>268</v>
       </c>
       <c r="B271" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="272" spans="1:2">
+      <c r="C271" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
       <c r="A272" t="s">
         <v>269</v>
       </c>
       <c r="B272" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="273" spans="1:2">
+      <c r="C272" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
       <c r="A273" t="s">
         <v>270</v>
       </c>
       <c r="B273" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="274" spans="1:2">
+      <c r="C273" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
       <c r="A274" t="s">
         <v>271</v>
       </c>
       <c r="B274" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="275" spans="1:2">
+      <c r="C274" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
       <c r="A275" t="s">
         <v>272</v>
       </c>
       <c r="B275" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="276" spans="1:2">
+      <c r="C275" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
       <c r="A276" t="s">
         <v>273</v>
       </c>
       <c r="B276" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="277" spans="1:2">
+      <c r="C276" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
       <c r="A277" t="s">
         <v>274</v>
       </c>
       <c r="B277" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="278" spans="1:2">
+      <c r="C277" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
       <c r="A278" t="s">
         <v>275</v>
       </c>
       <c r="B278" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="279" spans="1:2">
+      <c r="C278" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
       <c r="A279" t="s">
         <v>276</v>
       </c>
       <c r="B279" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="280" spans="1:2">
+      <c r="C279" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
       <c r="A280" t="s">
         <v>277</v>
       </c>
       <c r="B280" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="281" spans="1:2">
+      <c r="C280" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
       <c r="A281" t="s">
         <v>278</v>
       </c>
       <c r="B281" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="282" spans="1:2">
+      <c r="C281" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
       <c r="A282" t="s">
         <v>279</v>
       </c>
       <c r="B282" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="283" spans="1:2">
+      <c r="C282" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
       <c r="A283" t="s">
         <v>280</v>
       </c>
       <c r="B283" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="284" spans="1:2">
+      <c r="C283" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
       <c r="A284" t="s">
         <v>281</v>
       </c>
       <c r="B284" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="285" spans="1:2">
+      <c r="C284" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
       <c r="A285" t="s">
         <v>282</v>
       </c>
       <c r="B285" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="286" spans="1:2">
+      <c r="C285" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
       <c r="A286" t="s">
         <v>283</v>
       </c>
       <c r="B286" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="287" spans="1:2">
+      <c r="C286" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
       <c r="A287" t="s">
         <v>284</v>
       </c>
       <c r="B287" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="288" spans="1:2">
+      <c r="C287" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
       <c r="A288" t="s">
         <v>285</v>
       </c>
       <c r="B288" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="289" spans="1:2">
+      <c r="C288" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
       <c r="A289" t="s">
         <v>286</v>
       </c>
       <c r="B289" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="290" spans="1:2">
+      <c r="C289" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
       <c r="A290" t="s">
         <v>287</v>
       </c>
       <c r="B290" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="291" spans="1:2">
+      <c r="C290" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
       <c r="A291" t="s">
         <v>288</v>
       </c>
       <c r="B291" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="292" spans="1:2">
+      <c r="C291" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
       <c r="A292" t="s">
         <v>289</v>
       </c>
       <c r="B292" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="293" spans="1:2">
+      <c r="C292" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
       <c r="A293" t="s">
         <v>290</v>
       </c>
       <c r="B293" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="294" spans="1:2">
+      <c r="C293" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
       <c r="A294" t="s">
         <v>291</v>
       </c>
       <c r="B294" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="295" spans="1:2">
+      <c r="C294" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
       <c r="A295" t="s">
         <v>292</v>
       </c>
       <c r="B295" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="296" spans="1:2">
+      <c r="C295" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
       <c r="A296" t="s">
         <v>293</v>
       </c>
       <c r="B296" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="297" spans="1:2">
+      <c r="C296" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
       <c r="A297" t="s">
         <v>294</v>
       </c>
       <c r="B297" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="298" spans="1:2">
+      <c r="C297" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
       <c r="A298" t="s">
         <v>295</v>
       </c>
       <c r="B298" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="299" spans="1:2">
+      <c r="C298" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
       <c r="A299" t="s">
         <v>296</v>
       </c>
       <c r="B299" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="300" spans="1:2">
+      <c r="C299" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
       <c r="A300" t="s">
         <v>297</v>
       </c>
       <c r="B300" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="301" spans="1:2">
+      <c r="C300" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
       <c r="A301" t="s">
         <v>298</v>
       </c>
       <c r="B301" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="302" spans="1:2">
+      <c r="C301" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
       <c r="A302" t="s">
         <v>299</v>
       </c>
       <c r="B302" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="303" spans="1:2">
+      <c r="C302" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
       <c r="A303" t="s">
         <v>300</v>
       </c>
       <c r="B303" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="304" spans="1:2">
+      <c r="C303" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
       <c r="A304" t="s">
         <v>301</v>
       </c>
       <c r="B304" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="305" spans="1:2">
+      <c r="C304" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
       <c r="A305" t="s">
         <v>302</v>
       </c>
       <c r="B305" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="306" spans="1:2">
+      <c r="C305" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
       <c r="A306" t="s">
         <v>303</v>
       </c>
       <c r="B306" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="307" spans="1:2">
+      <c r="C306" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
       <c r="A307" t="s">
         <v>304</v>
       </c>
       <c r="B307" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="308" spans="1:2">
+      <c r="C307" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
       <c r="A308" t="s">
         <v>305</v>
       </c>
       <c r="B308" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="309" spans="1:2">
+      <c r="C308" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
       <c r="A309" t="s">
         <v>306</v>
       </c>
       <c r="B309" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="310" spans="1:2">
+      <c r="C309" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
       <c r="A310" t="s">
         <v>307</v>
       </c>
       <c r="B310" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="311" spans="1:2">
+      <c r="C310" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
       <c r="A311" t="s">
         <v>308</v>
       </c>
       <c r="B311" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="312" spans="1:2">
+      <c r="C311" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
       <c r="A312" t="s">
         <v>309</v>
       </c>
       <c r="B312" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="313" spans="1:2">
+      <c r="C312" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
       <c r="A313" t="s">
         <v>310</v>
       </c>
       <c r="B313" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="314" spans="1:2">
+      <c r="C313" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
       <c r="A314" t="s">
         <v>311</v>
       </c>
       <c r="B314" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="315" spans="1:2">
+      <c r="C314" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
       <c r="A315" t="s">
         <v>312</v>
       </c>
       <c r="B315" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="316" spans="1:2">
+      <c r="C315" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
       <c r="A316" t="s">
         <v>313</v>
       </c>
       <c r="B316" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="317" spans="1:2">
+      <c r="C316" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
       <c r="A317" t="s">
         <v>314</v>
       </c>
       <c r="B317" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="318" spans="1:2">
+      <c r="C317" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
       <c r="A318" t="s">
         <v>315</v>
       </c>
       <c r="B318" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="319" spans="1:2">
+      <c r="C318" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
       <c r="A319" t="s">
         <v>316</v>
       </c>
       <c r="B319" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="320" spans="1:2">
+      <c r="C319" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
       <c r="A320" t="s">
         <v>317</v>
       </c>
       <c r="B320" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="321" spans="1:2">
+      <c r="C320" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
       <c r="A321" t="s">
         <v>318</v>
       </c>
       <c r="B321" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="322" spans="1:2">
+      <c r="C321" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
       <c r="A322" t="s">
         <v>319</v>
       </c>
       <c r="B322" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="323" spans="1:2">
+      <c r="C322" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
       <c r="A323" t="s">
         <v>320</v>
       </c>
       <c r="B323" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="324" spans="1:2">
+      <c r="C323" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
       <c r="A324" t="s">
         <v>321</v>
       </c>
       <c r="B324" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="325" spans="1:2">
+      <c r="C324" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
       <c r="A325" t="s">
         <v>322</v>
       </c>
       <c r="B325" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="326" spans="1:2">
+      <c r="C325" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
       <c r="A326" t="s">
         <v>323</v>
       </c>
       <c r="B326" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="327" spans="1:2">
+      <c r="C326" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
       <c r="A327" s="4" t="s">
         <v>324</v>
       </c>
       <c r="B327" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="328" spans="1:2">
+      <c r="C327" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
       <c r="A328" t="s">
         <v>325</v>
       </c>
       <c r="B328" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="329" spans="1:2">
+      <c r="C328" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
       <c r="A329" t="s">
         <v>326</v>
       </c>
       <c r="B329" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="331" spans="1:2">
+      <c r="C329" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
       <c r="A331" s="1" t="s">
         <v>327</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Complete">
+  <conditionalFormatting sqref="B1:C1048576">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not started">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Not started">
       <formula>NOT(ISERROR(SEARCH("Not started",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Not porting">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Not porting">
       <formula>NOT(ISERROR(SEARCH("Not porting",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Down the Swift rabbit-hole
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="0" windowWidth="29060" windowHeight="18580" tabRatio="500"/>
+    <workbookView xWindow="13340" yWindow="0" windowWidth="20260" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="341">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1036,6 +1036,12 @@
   </si>
   <si>
     <t>Missing array return bug</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Revert to struct and replace forced packedlength once compiler support</t>
   </si>
 </sst>
 </file>
@@ -1093,235 +1099,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1706,25 +1484,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D331"/>
+  <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="2" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+    <row r="3" spans="1:5" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1735,15 +1513,18 @@
         <v>337</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
+    <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1753,8 +1534,11 @@
       <c r="C7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1764,8 +1548,11 @@
       <c r="C8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1775,8 +1562,11 @@
       <c r="C9" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1786,8 +1576,11 @@
       <c r="C10" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1797,8 +1590,11 @@
       <c r="C11" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1806,10 +1602,13 @@
         <v>328</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>328</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1819,8 +1618,11 @@
       <c r="C13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1830,8 +1632,11 @@
       <c r="C14" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1841,8 +1646,11 @@
       <c r="C15" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1850,10 +1658,16 @@
         <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>328</v>
+      </c>
+      <c r="D16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1861,21 +1675,24 @@
         <v>192</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>328</v>
+      </c>
+      <c r="D17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>192</v>
       </c>
-      <c r="C18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1885,8 +1702,11 @@
       <c r="C19" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1896,8 +1716,11 @@
       <c r="C20" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1907,8 +1730,11 @@
       <c r="C21" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1918,8 +1744,11 @@
       <c r="C22" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1929,8 +1758,11 @@
       <c r="C23" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1940,8 +1772,11 @@
       <c r="C24" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1951,8 +1786,11 @@
       <c r="C25" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1962,8 +1800,11 @@
       <c r="C26" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1973,8 +1814,11 @@
       <c r="C27" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1984,8 +1828,11 @@
       <c r="C28" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1995,8 +1842,11 @@
       <c r="C29" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2006,8 +1856,11 @@
       <c r="C30" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2017,8 +1870,11 @@
       <c r="C31" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2028,8 +1884,11 @@
       <c r="C32" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2039,8 +1898,11 @@
       <c r="C33" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2050,8 +1912,11 @@
       <c r="C34" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2061,8 +1926,11 @@
       <c r="C35" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2072,8 +1940,11 @@
       <c r="C36" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2083,8 +1954,11 @@
       <c r="C37" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2094,8 +1968,11 @@
       <c r="C38" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2105,8 +1982,11 @@
       <c r="C39" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2116,8 +1996,11 @@
       <c r="C40" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -2127,8 +2010,11 @@
       <c r="C41" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -2138,8 +2024,11 @@
       <c r="C42" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -2149,8 +2038,11 @@
       <c r="C43" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -2160,8 +2052,11 @@
       <c r="C44" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -2171,8 +2066,11 @@
       <c r="C45" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -2182,8 +2080,11 @@
       <c r="C46" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -2193,8 +2094,11 @@
       <c r="C47" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -2204,8 +2108,11 @@
       <c r="C48" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="D48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -2215,8 +2122,11 @@
       <c r="C49" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="D49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -2226,8 +2136,11 @@
       <c r="C50" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="D50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -2237,8 +2150,11 @@
       <c r="C51" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="D51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
@@ -2246,10 +2162,13 @@
         <v>328</v>
       </c>
       <c r="D52" t="s">
+        <v>191</v>
+      </c>
+      <c r="E52" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -2259,8 +2178,11 @@
       <c r="C53" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="D53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -2270,8 +2192,11 @@
       <c r="C54" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="D54" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2281,8 +2206,11 @@
       <c r="C55" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="D55" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -2292,8 +2220,11 @@
       <c r="C56" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="D56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2303,8 +2234,11 @@
       <c r="C57" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="D57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -2314,8 +2248,11 @@
       <c r="C58" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="D58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -2325,8 +2262,11 @@
       <c r="C59" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="D59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -2336,8 +2276,11 @@
       <c r="C60" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="D60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -2347,8 +2290,11 @@
       <c r="C61" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="D61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
@@ -2358,8 +2304,11 @@
       <c r="C62" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="D62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
@@ -2369,8 +2318,11 @@
       <c r="C63" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="D63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -2380,8 +2332,11 @@
       <c r="C64" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -2391,8 +2346,11 @@
       <c r="C65" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -2402,8 +2360,11 @@
       <c r="C66" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
@@ -2413,8 +2374,11 @@
       <c r="C67" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
@@ -2424,8 +2388,11 @@
       <c r="C68" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
@@ -2435,8 +2402,11 @@
       <c r="C69" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
@@ -2446,8 +2416,11 @@
       <c r="C70" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
@@ -2457,8 +2430,11 @@
       <c r="C71" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -2468,8 +2444,11 @@
       <c r="C72" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
@@ -2479,8 +2458,11 @@
       <c r="C73" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -2490,8 +2472,11 @@
       <c r="C74" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -2501,8 +2486,11 @@
       <c r="C75" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
@@ -2512,8 +2500,11 @@
       <c r="C76" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
@@ -2523,8 +2514,11 @@
       <c r="C77" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -2534,8 +2528,11 @@
       <c r="C78" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
@@ -2545,8 +2542,11 @@
       <c r="C79" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -2556,16 +2556,22 @@
       <c r="C80" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="D80" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C81" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="D81" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -2575,8 +2581,11 @@
       <c r="C82" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="D82" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
@@ -2586,8 +2595,11 @@
       <c r="C83" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="D83" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
@@ -2597,8 +2609,11 @@
       <c r="C84" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="D84" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
@@ -2608,8 +2623,11 @@
       <c r="C85" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="D85" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -2619,8 +2637,11 @@
       <c r="C86" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="D86" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -2630,8 +2651,11 @@
       <c r="C87" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="D87" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -2641,8 +2665,11 @@
       <c r="C88" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="D88" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
@@ -2652,8 +2679,11 @@
       <c r="C89" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="D89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -2663,8 +2693,11 @@
       <c r="C90" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="D90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
@@ -2674,8 +2707,11 @@
       <c r="C91" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="D91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
@@ -2686,10 +2722,13 @@
         <v>191</v>
       </c>
       <c r="D92" t="s">
+        <v>191</v>
+      </c>
+      <c r="E92" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -2699,8 +2738,11 @@
       <c r="C93" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="D93" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
@@ -2710,8 +2752,11 @@
       <c r="C94" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
@@ -2721,8 +2766,11 @@
       <c r="C95" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="D95" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -2732,8 +2780,11 @@
       <c r="C96" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
@@ -2743,8 +2794,11 @@
       <c r="C97" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
@@ -2754,8 +2808,11 @@
       <c r="C98" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
@@ -2765,8 +2822,11 @@
       <c r="C99" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -2776,8 +2836,11 @@
       <c r="C100" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
@@ -2787,8 +2850,11 @@
       <c r="C101" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -2798,8 +2864,11 @@
       <c r="C102" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="D102" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
@@ -2809,8 +2878,11 @@
       <c r="C103" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
@@ -2820,8 +2892,11 @@
       <c r="C104" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="D104" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
@@ -2831,8 +2906,11 @@
       <c r="C105" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="D105" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
@@ -2842,8 +2920,11 @@
       <c r="C106" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
@@ -2853,8 +2934,11 @@
       <c r="C107" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
@@ -2864,8 +2948,11 @@
       <c r="C108" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="D108" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
@@ -2875,8 +2962,11 @@
       <c r="C109" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="D109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
         <v>108</v>
       </c>
@@ -2886,8 +2976,11 @@
       <c r="C110" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="D110" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
         <v>109</v>
       </c>
@@ -2897,8 +2990,11 @@
       <c r="C111" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
         <v>110</v>
       </c>
@@ -2908,8 +3004,11 @@
       <c r="C112" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="D112" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="2" t="s">
         <v>111</v>
       </c>
@@ -2920,10 +3019,13 @@
         <v>191</v>
       </c>
       <c r="D113" t="s">
+        <v>191</v>
+      </c>
+      <c r="E113" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114" s="2" t="s">
         <v>112</v>
       </c>
@@ -2933,8 +3035,11 @@
       <c r="C114" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="D114" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="2" t="s">
         <v>113</v>
       </c>
@@ -2944,8 +3049,11 @@
       <c r="C115" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="D115" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="2" t="s">
         <v>114</v>
       </c>
@@ -2955,8 +3063,11 @@
       <c r="C116" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="D116" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
@@ -2966,8 +3077,11 @@
       <c r="C117" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="D117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="2" t="s">
         <v>116</v>
       </c>
@@ -2977,8 +3091,11 @@
       <c r="C118" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="D118" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="2" t="s">
         <v>117</v>
       </c>
@@ -2988,8 +3105,11 @@
       <c r="C119" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="D119" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="2" t="s">
         <v>118</v>
       </c>
@@ -2999,8 +3119,11 @@
       <c r="C120" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="D120" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="2" t="s">
         <v>119</v>
       </c>
@@ -3010,8 +3133,11 @@
       <c r="C121" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="D121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="2" t="s">
         <v>120</v>
       </c>
@@ -3021,8 +3147,11 @@
       <c r="C122" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="D122" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="2" t="s">
         <v>121</v>
       </c>
@@ -3032,8 +3161,11 @@
       <c r="C123" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="D123" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="2" t="s">
         <v>122</v>
       </c>
@@ -3043,8 +3175,11 @@
       <c r="C124" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="D124" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="2" t="s">
         <v>123</v>
       </c>
@@ -3054,8 +3189,11 @@
       <c r="C125" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="D125" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="2" t="s">
         <v>124</v>
       </c>
@@ -3065,8 +3203,11 @@
       <c r="C126" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="D126" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="2" t="s">
         <v>125</v>
       </c>
@@ -3076,8 +3217,11 @@
       <c r="C127" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="D127" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="2" t="s">
         <v>126</v>
       </c>
@@ -3087,8 +3231,11 @@
       <c r="C128" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="2" t="s">
         <v>127</v>
       </c>
@@ -3098,8 +3245,11 @@
       <c r="C129" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="2" t="s">
         <v>128</v>
       </c>
@@ -3107,10 +3257,13 @@
         <v>192</v>
       </c>
       <c r="C130" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+        <v>328</v>
+      </c>
+      <c r="D130" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="2" t="s">
         <v>129</v>
       </c>
@@ -3120,8 +3273,11 @@
       <c r="C131" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="D131" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="2" t="s">
         <v>130</v>
       </c>
@@ -3131,8 +3287,11 @@
       <c r="C132" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="D132" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="2" t="s">
         <v>131</v>
       </c>
@@ -3142,8 +3301,11 @@
       <c r="C133" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="2" t="s">
         <v>132</v>
       </c>
@@ -3153,8 +3315,11 @@
       <c r="C134" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="2" t="s">
         <v>133</v>
       </c>
@@ -3164,8 +3329,11 @@
       <c r="C135" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="D135" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
         <v>134</v>
       </c>
@@ -3175,8 +3343,11 @@
       <c r="C136" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="D136" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
         <v>135</v>
       </c>
@@ -3186,8 +3357,11 @@
       <c r="C137" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="D137" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="2" t="s">
         <v>136</v>
       </c>
@@ -3197,8 +3371,11 @@
       <c r="C138" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="D138" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
         <v>137</v>
       </c>
@@ -3208,8 +3385,11 @@
       <c r="C139" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="D139" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="2" t="s">
         <v>138</v>
       </c>
@@ -3219,8 +3399,11 @@
       <c r="C140" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="D140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="2" t="s">
         <v>139</v>
       </c>
@@ -3230,8 +3413,11 @@
       <c r="C141" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="D141" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="2" t="s">
         <v>140</v>
       </c>
@@ -3241,8 +3427,11 @@
       <c r="C142" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="2" t="s">
         <v>141</v>
       </c>
@@ -3252,8 +3441,11 @@
       <c r="C143" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="D143" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="2" t="s">
         <v>142</v>
       </c>
@@ -3263,8 +3455,11 @@
       <c r="C144" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="D144" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="2" t="s">
         <v>143</v>
       </c>
@@ -3274,8 +3469,11 @@
       <c r="C145" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="D145" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="2" t="s">
         <v>144</v>
       </c>
@@ -3285,8 +3483,11 @@
       <c r="C146" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="D146" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="2" t="s">
         <v>145</v>
       </c>
@@ -3296,8 +3497,11 @@
       <c r="C147" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="D147" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="2" t="s">
         <v>146</v>
       </c>
@@ -3307,8 +3511,11 @@
       <c r="C148" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="D148" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="2" t="s">
         <v>147</v>
       </c>
@@ -3318,8 +3525,11 @@
       <c r="C149" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="D149" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="2" t="s">
         <v>148</v>
       </c>
@@ -3329,8 +3539,11 @@
       <c r="C150" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="D150" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -3340,8 +3553,11 @@
       <c r="C151" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="D151" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -3351,8 +3567,11 @@
       <c r="C152" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="D152" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -3362,8 +3581,11 @@
       <c r="C153" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="D153" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" s="2" t="s">
         <v>152</v>
       </c>
@@ -3373,8 +3595,11 @@
       <c r="C154" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="D154" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" s="2" t="s">
         <v>153</v>
       </c>
@@ -3384,8 +3609,11 @@
       <c r="C155" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="D155" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" s="2" t="s">
         <v>154</v>
       </c>
@@ -3395,8 +3623,11 @@
       <c r="C156" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="D156" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" s="2" t="s">
         <v>155</v>
       </c>
@@ -3406,8 +3637,11 @@
       <c r="C157" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="D157" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" s="2" t="s">
         <v>156</v>
       </c>
@@ -3418,10 +3652,13 @@
         <v>191</v>
       </c>
       <c r="D158" t="s">
+        <v>191</v>
+      </c>
+      <c r="E158" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:5">
       <c r="A159" s="2" t="s">
         <v>157</v>
       </c>
@@ -3432,10 +3669,13 @@
         <v>191</v>
       </c>
       <c r="D159" t="s">
+        <v>191</v>
+      </c>
+      <c r="E159" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:5">
       <c r="A160" s="2" t="s">
         <v>158</v>
       </c>
@@ -3446,21 +3686,24 @@
         <v>191</v>
       </c>
       <c r="D160" t="s">
+        <v>191</v>
+      </c>
+      <c r="E160" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:5">
       <c r="A161" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B161" t="s">
-        <v>190</v>
-      </c>
       <c r="C161" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+        <v>192</v>
+      </c>
+      <c r="D161" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" s="2" t="s">
         <v>160</v>
       </c>
@@ -3470,8 +3713,11 @@
       <c r="C162" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="D162" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" s="2" t="s">
         <v>161</v>
       </c>
@@ -3481,8 +3727,11 @@
       <c r="C163" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="D163" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" s="2" t="s">
         <v>162</v>
       </c>
@@ -3492,8 +3741,11 @@
       <c r="C164" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="D164" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" s="2" t="s">
         <v>163</v>
       </c>
@@ -3503,8 +3755,11 @@
       <c r="C165" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="D165" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" s="2" t="s">
         <v>164</v>
       </c>
@@ -3514,8 +3769,11 @@
       <c r="C166" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="D166" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167" s="2" t="s">
         <v>165</v>
       </c>
@@ -3526,10 +3784,13 @@
         <v>191</v>
       </c>
       <c r="D167" t="s">
+        <v>191</v>
+      </c>
+      <c r="E167" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:5">
       <c r="A168" s="2" t="s">
         <v>166</v>
       </c>
@@ -3539,8 +3800,11 @@
       <c r="C168" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="D168" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" s="2" t="s">
         <v>167</v>
       </c>
@@ -3550,8 +3814,11 @@
       <c r="C169" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="D169" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" s="2" t="s">
         <v>168</v>
       </c>
@@ -3561,8 +3828,11 @@
       <c r="C170" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="D170" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" s="2" t="s">
         <v>169</v>
       </c>
@@ -3572,8 +3842,11 @@
       <c r="C171" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="D171" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="2" t="s">
         <v>170</v>
       </c>
@@ -3583,8 +3856,11 @@
       <c r="C172" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="D172" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" s="2" t="s">
         <v>171</v>
       </c>
@@ -3594,8 +3870,11 @@
       <c r="C173" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="D173" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174" s="2" t="s">
         <v>172</v>
       </c>
@@ -3605,8 +3884,11 @@
       <c r="C174" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="D174" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" s="2" t="s">
         <v>173</v>
       </c>
@@ -3616,8 +3898,11 @@
       <c r="C175" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="D175" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" s="2" t="s">
         <v>174</v>
       </c>
@@ -3627,8 +3912,11 @@
       <c r="C176" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="177" spans="1:3">
+      <c r="D176" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="2" t="s">
         <v>175</v>
       </c>
@@ -3638,8 +3926,11 @@
       <c r="C177" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="D177" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="2" t="s">
         <v>176</v>
       </c>
@@ -3649,8 +3940,11 @@
       <c r="C178" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="179" spans="1:3">
+      <c r="D178" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" s="2" t="s">
         <v>177</v>
       </c>
@@ -3660,8 +3954,11 @@
       <c r="C179" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="180" spans="1:3">
+      <c r="D179" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="2" t="s">
         <v>178</v>
       </c>
@@ -3671,8 +3968,11 @@
       <c r="C180" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="181" spans="1:3">
+      <c r="D180" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="2" t="s">
         <v>179</v>
       </c>
@@ -3682,8 +3982,11 @@
       <c r="C181" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="182" spans="1:3">
+      <c r="D181" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="2" t="s">
         <v>180</v>
       </c>
@@ -3693,8 +3996,11 @@
       <c r="C182" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="183" spans="1:3">
+      <c r="D182" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="2" t="s">
         <v>181</v>
       </c>
@@ -3704,8 +4010,11 @@
       <c r="C183" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="184" spans="1:3">
+      <c r="D183" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" s="2" t="s">
         <v>182</v>
       </c>
@@ -3715,8 +4024,11 @@
       <c r="C184" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="185" spans="1:3">
+      <c r="D184" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" s="2" t="s">
         <v>183</v>
       </c>
@@ -3726,8 +4038,11 @@
       <c r="C185" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="186" spans="1:3">
+      <c r="D185" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
@@ -3737,8 +4052,11 @@
       <c r="C186" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="187" spans="1:3">
+      <c r="D186" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="2" t="s">
         <v>185</v>
       </c>
@@ -3748,8 +4066,11 @@
       <c r="C187" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="188" spans="1:3">
+      <c r="D187" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="2" t="s">
         <v>186</v>
       </c>
@@ -3759,8 +4080,11 @@
       <c r="C188" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="189" spans="1:3">
+      <c r="D188" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="2" t="s">
         <v>187</v>
       </c>
@@ -3770,8 +4094,11 @@
       <c r="C189" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="190" spans="1:3">
+      <c r="D189" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="2" t="s">
         <v>188</v>
       </c>
@@ -3781,8 +4108,11 @@
       <c r="C190" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="191" spans="1:3">
+      <c r="D190" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="2" t="s">
         <v>189</v>
       </c>
@@ -3792,13 +4122,16 @@
       <c r="C191" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="D191" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
       <c r="A193" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -3808,8 +4141,11 @@
       <c r="C195" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="D195" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -3819,8 +4155,11 @@
       <c r="C196" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="D196" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -3830,8 +4169,11 @@
       <c r="C197" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="D197" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -3841,8 +4183,11 @@
       <c r="C198" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="D198" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -3852,8 +4197,11 @@
       <c r="C199" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="D199" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -3863,8 +4211,11 @@
       <c r="C200" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="D200" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -3874,8 +4225,11 @@
       <c r="C201" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="202" spans="1:4">
+      <c r="D201" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3886,10 +4240,13 @@
         <v>191</v>
       </c>
       <c r="D202" t="s">
+        <v>191</v>
+      </c>
+      <c r="E202" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -3899,8 +4256,11 @@
       <c r="C203" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="D203" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -3910,8 +4270,11 @@
       <c r="C204" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="D204" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3922,10 +4285,13 @@
         <v>191</v>
       </c>
       <c r="D205" t="s">
+        <v>191</v>
+      </c>
+      <c r="E205" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3935,8 +4301,11 @@
       <c r="C206" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="D206" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3946,8 +4315,11 @@
       <c r="C207" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="D207" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3958,10 +4330,13 @@
         <v>191</v>
       </c>
       <c r="D208" t="s">
+        <v>191</v>
+      </c>
+      <c r="E208" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3971,8 +4346,11 @@
       <c r="C209" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="210" spans="1:4">
+      <c r="D209" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3982,8 +4360,11 @@
       <c r="C210" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="211" spans="1:4">
+      <c r="D210" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3993,8 +4374,11 @@
       <c r="C211" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="212" spans="1:4">
+      <c r="D211" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -4004,8 +4388,11 @@
       <c r="C212" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="213" spans="1:4">
+      <c r="D212" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -4015,8 +4402,11 @@
       <c r="C213" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="214" spans="1:4">
+      <c r="D213" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -4026,8 +4416,11 @@
       <c r="C214" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="215" spans="1:4">
+      <c r="D214" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -4037,8 +4430,11 @@
       <c r="C215" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="D215" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -4048,8 +4444,11 @@
       <c r="C216" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="217" spans="1:4">
+      <c r="D216" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -4059,8 +4458,11 @@
       <c r="C217" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="218" spans="1:4">
+      <c r="D217" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -4071,10 +4473,13 @@
         <v>191</v>
       </c>
       <c r="D218" t="s">
+        <v>191</v>
+      </c>
+      <c r="E218" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -4084,8 +4489,11 @@
       <c r="C219" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="220" spans="1:4">
+      <c r="D219" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -4095,8 +4503,11 @@
       <c r="C220" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="221" spans="1:4">
+      <c r="D220" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -4106,8 +4517,11 @@
       <c r="C221" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="222" spans="1:4">
+      <c r="D221" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -4117,13 +4531,16 @@
       <c r="C222" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="224" spans="1:4">
+      <c r="D222" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>223</v>
       </c>
@@ -4133,8 +4550,11 @@
       <c r="C226" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="227" spans="1:3">
+      <c r="D226" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>224</v>
       </c>
@@ -4144,8 +4564,11 @@
       <c r="C227" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="228" spans="1:3">
+      <c r="D227" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>225</v>
       </c>
@@ -4155,8 +4578,11 @@
       <c r="C228" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="229" spans="1:3">
+      <c r="D228" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>226</v>
       </c>
@@ -4166,8 +4592,11 @@
       <c r="C229" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="230" spans="1:3">
+      <c r="D229" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>227</v>
       </c>
@@ -4177,8 +4606,11 @@
       <c r="C230" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="231" spans="1:3">
+      <c r="D230" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>228</v>
       </c>
@@ -4188,8 +4620,11 @@
       <c r="C231" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="232" spans="1:3">
+      <c r="D231" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>229</v>
       </c>
@@ -4199,8 +4634,11 @@
       <c r="C232" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="233" spans="1:3">
+      <c r="D232" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>230</v>
       </c>
@@ -4210,8 +4648,11 @@
       <c r="C233" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="234" spans="1:3">
+      <c r="D233" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>231</v>
       </c>
@@ -4221,8 +4662,11 @@
       <c r="C234" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="235" spans="1:3">
+      <c r="D234" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>232</v>
       </c>
@@ -4232,8 +4676,11 @@
       <c r="C235" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="236" spans="1:3">
+      <c r="D235" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>233</v>
       </c>
@@ -4243,8 +4690,11 @@
       <c r="C236" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="237" spans="1:3">
+      <c r="D236" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>234</v>
       </c>
@@ -4254,8 +4704,11 @@
       <c r="C237" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="238" spans="1:3">
+      <c r="D237" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>235</v>
       </c>
@@ -4265,8 +4718,11 @@
       <c r="C238" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="239" spans="1:3">
+      <c r="D238" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>236</v>
       </c>
@@ -4276,8 +4732,11 @@
       <c r="C239" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="240" spans="1:3">
+      <c r="D239" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>237</v>
       </c>
@@ -4287,8 +4746,11 @@
       <c r="C240" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="241" spans="1:3">
+      <c r="D240" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>238</v>
       </c>
@@ -4298,8 +4760,11 @@
       <c r="C241" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="242" spans="1:3">
+      <c r="D241" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>239</v>
       </c>
@@ -4309,8 +4774,11 @@
       <c r="C242" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="243" spans="1:3">
+      <c r="D242" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
       <c r="A243" t="s">
         <v>240</v>
       </c>
@@ -4320,8 +4788,11 @@
       <c r="C243" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="244" spans="1:3">
+      <c r="D243" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
       <c r="A244" t="s">
         <v>241</v>
       </c>
@@ -4331,8 +4802,11 @@
       <c r="C244" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="245" spans="1:3">
+      <c r="D244" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
       <c r="A245" t="s">
         <v>242</v>
       </c>
@@ -4342,8 +4816,11 @@
       <c r="C245" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="246" spans="1:3">
+      <c r="D245" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
       <c r="A246" t="s">
         <v>243</v>
       </c>
@@ -4353,8 +4830,11 @@
       <c r="C246" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="247" spans="1:3">
+      <c r="D246" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
       <c r="A247" t="s">
         <v>244</v>
       </c>
@@ -4364,8 +4844,11 @@
       <c r="C247" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="248" spans="1:3">
+      <c r="D247" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
       <c r="A248" t="s">
         <v>245</v>
       </c>
@@ -4375,8 +4858,11 @@
       <c r="C248" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="249" spans="1:3">
+      <c r="D248" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
       <c r="A249" t="s">
         <v>246</v>
       </c>
@@ -4386,8 +4872,11 @@
       <c r="C249" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="250" spans="1:3">
+      <c r="D249" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
       <c r="A250" t="s">
         <v>247</v>
       </c>
@@ -4397,8 +4886,11 @@
       <c r="C250" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="251" spans="1:3">
+      <c r="D250" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
       <c r="A251" t="s">
         <v>248</v>
       </c>
@@ -4408,8 +4900,11 @@
       <c r="C251" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="252" spans="1:3">
+      <c r="D251" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
       <c r="A252" t="s">
         <v>249</v>
       </c>
@@ -4419,8 +4914,11 @@
       <c r="C252" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="253" spans="1:3">
+      <c r="D252" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
       <c r="A253" t="s">
         <v>250</v>
       </c>
@@ -4430,8 +4928,11 @@
       <c r="C253" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="254" spans="1:3">
+      <c r="D253" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
       <c r="A254" t="s">
         <v>251</v>
       </c>
@@ -4441,8 +4942,11 @@
       <c r="C254" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="255" spans="1:3">
+      <c r="D254" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
       <c r="A255" t="s">
         <v>252</v>
       </c>
@@ -4452,8 +4956,11 @@
       <c r="C255" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="256" spans="1:3">
+      <c r="D255" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
       <c r="A256" t="s">
         <v>253</v>
       </c>
@@ -4463,8 +4970,11 @@
       <c r="C256" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="257" spans="1:3">
+      <c r="D256" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
       <c r="A257" t="s">
         <v>254</v>
       </c>
@@ -4474,8 +4984,11 @@
       <c r="C257" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="258" spans="1:3">
+      <c r="D257" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
       <c r="A258" t="s">
         <v>255</v>
       </c>
@@ -4485,8 +4998,11 @@
       <c r="C258" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="259" spans="1:3">
+      <c r="D258" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
       <c r="A259" t="s">
         <v>256</v>
       </c>
@@ -4496,8 +5012,11 @@
       <c r="C259" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="260" spans="1:3">
+      <c r="D259" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
       <c r="A260" t="s">
         <v>257</v>
       </c>
@@ -4507,8 +5026,11 @@
       <c r="C260" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="261" spans="1:3">
+      <c r="D260" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
       <c r="A261" t="s">
         <v>258</v>
       </c>
@@ -4518,8 +5040,11 @@
       <c r="C261" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="262" spans="1:3">
+      <c r="D261" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
       <c r="A262" t="s">
         <v>259</v>
       </c>
@@ -4529,8 +5054,11 @@
       <c r="C262" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="263" spans="1:3">
+      <c r="D262" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
       <c r="A263" t="s">
         <v>260</v>
       </c>
@@ -4540,8 +5068,11 @@
       <c r="C263" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="264" spans="1:3">
+      <c r="D263" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
       <c r="A264" t="s">
         <v>261</v>
       </c>
@@ -4551,8 +5082,11 @@
       <c r="C264" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="265" spans="1:3">
+      <c r="D264" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
       <c r="A265" t="s">
         <v>262</v>
       </c>
@@ -4562,8 +5096,11 @@
       <c r="C265" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="266" spans="1:3">
+      <c r="D265" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
       <c r="A266" t="s">
         <v>263</v>
       </c>
@@ -4573,8 +5110,11 @@
       <c r="C266" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="267" spans="1:3">
+      <c r="D266" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
       <c r="A267" t="s">
         <v>264</v>
       </c>
@@ -4584,8 +5124,11 @@
       <c r="C267" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="268" spans="1:3">
+      <c r="D267" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
       <c r="A268" t="s">
         <v>265</v>
       </c>
@@ -4595,8 +5138,11 @@
       <c r="C268" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="269" spans="1:3">
+      <c r="D268" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
       <c r="A269" t="s">
         <v>266</v>
       </c>
@@ -4606,8 +5152,11 @@
       <c r="C269" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="270" spans="1:3">
+      <c r="D269" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
       <c r="A270" t="s">
         <v>267</v>
       </c>
@@ -4617,8 +5166,11 @@
       <c r="C270" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="271" spans="1:3">
+      <c r="D270" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
       <c r="A271" t="s">
         <v>268</v>
       </c>
@@ -4628,8 +5180,11 @@
       <c r="C271" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="272" spans="1:3">
+      <c r="D271" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
       <c r="A272" t="s">
         <v>269</v>
       </c>
@@ -4639,8 +5194,11 @@
       <c r="C272" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="273" spans="1:3">
+      <c r="D272" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4">
       <c r="A273" t="s">
         <v>270</v>
       </c>
@@ -4650,8 +5208,11 @@
       <c r="C273" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="274" spans="1:3">
+      <c r="D273" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
       <c r="A274" t="s">
         <v>271</v>
       </c>
@@ -4661,8 +5222,11 @@
       <c r="C274" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="275" spans="1:3">
+      <c r="D274" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
       <c r="A275" t="s">
         <v>272</v>
       </c>
@@ -4672,8 +5236,11 @@
       <c r="C275" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="276" spans="1:3">
+      <c r="D275" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
       <c r="A276" t="s">
         <v>273</v>
       </c>
@@ -4683,8 +5250,11 @@
       <c r="C276" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="277" spans="1:3">
+      <c r="D276" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
       <c r="A277" t="s">
         <v>274</v>
       </c>
@@ -4694,8 +5264,11 @@
       <c r="C277" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="278" spans="1:3">
+      <c r="D277" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
       <c r="A278" t="s">
         <v>275</v>
       </c>
@@ -4705,8 +5278,11 @@
       <c r="C278" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="279" spans="1:3">
+      <c r="D278" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
       <c r="A279" t="s">
         <v>276</v>
       </c>
@@ -4716,8 +5292,11 @@
       <c r="C279" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="280" spans="1:3">
+      <c r="D279" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
       <c r="A280" t="s">
         <v>277</v>
       </c>
@@ -4727,8 +5306,11 @@
       <c r="C280" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="281" spans="1:3">
+      <c r="D280" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
       <c r="A281" t="s">
         <v>278</v>
       </c>
@@ -4738,8 +5320,11 @@
       <c r="C281" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="282" spans="1:3">
+      <c r="D281" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
       <c r="A282" t="s">
         <v>279</v>
       </c>
@@ -4749,8 +5334,11 @@
       <c r="C282" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="283" spans="1:3">
+      <c r="D282" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
       <c r="A283" t="s">
         <v>280</v>
       </c>
@@ -4760,8 +5348,11 @@
       <c r="C283" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="284" spans="1:3">
+      <c r="D283" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
       <c r="A284" t="s">
         <v>281</v>
       </c>
@@ -4771,8 +5362,11 @@
       <c r="C284" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="285" spans="1:3">
+      <c r="D284" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
       <c r="A285" t="s">
         <v>282</v>
       </c>
@@ -4782,8 +5376,11 @@
       <c r="C285" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="286" spans="1:3">
+      <c r="D285" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
       <c r="A286" t="s">
         <v>283</v>
       </c>
@@ -4793,8 +5390,11 @@
       <c r="C286" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="287" spans="1:3">
+      <c r="D286" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
       <c r="A287" t="s">
         <v>284</v>
       </c>
@@ -4804,8 +5404,11 @@
       <c r="C287" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="288" spans="1:3">
+      <c r="D287" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
       <c r="A288" t="s">
         <v>285</v>
       </c>
@@ -4815,8 +5418,11 @@
       <c r="C288" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="289" spans="1:3">
+      <c r="D288" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
       <c r="A289" t="s">
         <v>286</v>
       </c>
@@ -4826,8 +5432,11 @@
       <c r="C289" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="290" spans="1:3">
+      <c r="D289" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
       <c r="A290" t="s">
         <v>287</v>
       </c>
@@ -4837,8 +5446,11 @@
       <c r="C290" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="291" spans="1:3">
+      <c r="D290" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
       <c r="A291" t="s">
         <v>288</v>
       </c>
@@ -4848,8 +5460,11 @@
       <c r="C291" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="292" spans="1:3">
+      <c r="D291" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
       <c r="A292" t="s">
         <v>289</v>
       </c>
@@ -4859,8 +5474,11 @@
       <c r="C292" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="293" spans="1:3">
+      <c r="D292" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
       <c r="A293" t="s">
         <v>290</v>
       </c>
@@ -4870,8 +5488,11 @@
       <c r="C293" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="294" spans="1:3">
+      <c r="D293" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
       <c r="A294" t="s">
         <v>291</v>
       </c>
@@ -4881,8 +5502,11 @@
       <c r="C294" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="295" spans="1:3">
+      <c r="D294" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4">
       <c r="A295" t="s">
         <v>292</v>
       </c>
@@ -4892,8 +5516,11 @@
       <c r="C295" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="296" spans="1:3">
+      <c r="D295" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
       <c r="A296" t="s">
         <v>293</v>
       </c>
@@ -4903,8 +5530,11 @@
       <c r="C296" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="297" spans="1:3">
+      <c r="D296" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
       <c r="A297" t="s">
         <v>294</v>
       </c>
@@ -4914,8 +5544,11 @@
       <c r="C297" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="298" spans="1:3">
+      <c r="D297" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
       <c r="A298" t="s">
         <v>295</v>
       </c>
@@ -4925,8 +5558,11 @@
       <c r="C298" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="299" spans="1:3">
+      <c r="D298" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
       <c r="A299" t="s">
         <v>296</v>
       </c>
@@ -4936,8 +5572,11 @@
       <c r="C299" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="300" spans="1:3">
+      <c r="D299" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
       <c r="A300" t="s">
         <v>297</v>
       </c>
@@ -4947,8 +5586,11 @@
       <c r="C300" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="301" spans="1:3">
+      <c r="D300" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
       <c r="A301" t="s">
         <v>298</v>
       </c>
@@ -4958,8 +5600,11 @@
       <c r="C301" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="302" spans="1:3">
+      <c r="D301" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
       <c r="A302" t="s">
         <v>299</v>
       </c>
@@ -4969,8 +5614,11 @@
       <c r="C302" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="303" spans="1:3">
+      <c r="D302" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
       <c r="A303" t="s">
         <v>300</v>
       </c>
@@ -4980,8 +5628,11 @@
       <c r="C303" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="304" spans="1:3">
+      <c r="D303" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
       <c r="A304" t="s">
         <v>301</v>
       </c>
@@ -4991,8 +5642,11 @@
       <c r="C304" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="305" spans="1:3">
+      <c r="D304" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
       <c r="A305" t="s">
         <v>302</v>
       </c>
@@ -5002,8 +5656,11 @@
       <c r="C305" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="306" spans="1:3">
+      <c r="D305" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
       <c r="A306" t="s">
         <v>303</v>
       </c>
@@ -5013,8 +5670,11 @@
       <c r="C306" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="307" spans="1:3">
+      <c r="D306" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
       <c r="A307" t="s">
         <v>304</v>
       </c>
@@ -5024,8 +5684,11 @@
       <c r="C307" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="308" spans="1:3">
+      <c r="D307" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4">
       <c r="A308" t="s">
         <v>305</v>
       </c>
@@ -5035,8 +5698,11 @@
       <c r="C308" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="309" spans="1:3">
+      <c r="D308" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
       <c r="A309" t="s">
         <v>306</v>
       </c>
@@ -5046,8 +5712,11 @@
       <c r="C309" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="310" spans="1:3">
+      <c r="D309" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
       <c r="A310" t="s">
         <v>307</v>
       </c>
@@ -5057,8 +5726,11 @@
       <c r="C310" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="311" spans="1:3">
+      <c r="D310" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
       <c r="A311" t="s">
         <v>308</v>
       </c>
@@ -5068,8 +5740,11 @@
       <c r="C311" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="312" spans="1:3">
+      <c r="D311" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
       <c r="A312" t="s">
         <v>309</v>
       </c>
@@ -5079,8 +5754,11 @@
       <c r="C312" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="313" spans="1:3">
+      <c r="D312" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
       <c r="A313" t="s">
         <v>310</v>
       </c>
@@ -5090,8 +5768,11 @@
       <c r="C313" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="314" spans="1:3">
+      <c r="D313" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
       <c r="A314" t="s">
         <v>311</v>
       </c>
@@ -5101,8 +5782,11 @@
       <c r="C314" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="315" spans="1:3">
+      <c r="D314" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
       <c r="A315" t="s">
         <v>312</v>
       </c>
@@ -5112,8 +5796,11 @@
       <c r="C315" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="316" spans="1:3">
+      <c r="D315" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
       <c r="A316" t="s">
         <v>313</v>
       </c>
@@ -5123,8 +5810,11 @@
       <c r="C316" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="317" spans="1:3">
+      <c r="D316" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4">
       <c r="A317" t="s">
         <v>314</v>
       </c>
@@ -5134,8 +5824,11 @@
       <c r="C317" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="318" spans="1:3">
+      <c r="D317" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4">
       <c r="A318" t="s">
         <v>315</v>
       </c>
@@ -5145,8 +5838,11 @@
       <c r="C318" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="319" spans="1:3">
+      <c r="D318" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
       <c r="A319" t="s">
         <v>316</v>
       </c>
@@ -5156,8 +5852,11 @@
       <c r="C319" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="320" spans="1:3">
+      <c r="D319" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4">
       <c r="A320" t="s">
         <v>317</v>
       </c>
@@ -5167,8 +5866,11 @@
       <c r="C320" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="321" spans="1:3">
+      <c r="D320" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4">
       <c r="A321" t="s">
         <v>318</v>
       </c>
@@ -5178,8 +5880,11 @@
       <c r="C321" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="322" spans="1:3">
+      <c r="D321" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4">
       <c r="A322" t="s">
         <v>319</v>
       </c>
@@ -5189,8 +5894,11 @@
       <c r="C322" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="323" spans="1:3">
+      <c r="D322" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4">
       <c r="A323" t="s">
         <v>320</v>
       </c>
@@ -5200,8 +5908,11 @@
       <c r="C323" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="324" spans="1:3">
+      <c r="D323" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4">
       <c r="A324" t="s">
         <v>321</v>
       </c>
@@ -5211,8 +5922,11 @@
       <c r="C324" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="325" spans="1:3">
+      <c r="D324" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4">
       <c r="A325" t="s">
         <v>322</v>
       </c>
@@ -5222,8 +5936,11 @@
       <c r="C325" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="326" spans="1:3">
+      <c r="D325" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4">
       <c r="A326" t="s">
         <v>323</v>
       </c>
@@ -5233,8 +5950,11 @@
       <c r="C326" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="327" spans="1:3">
+      <c r="D326" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4">
       <c r="A327" s="4" t="s">
         <v>324</v>
       </c>
@@ -5244,8 +5964,11 @@
       <c r="C327" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="328" spans="1:3">
+      <c r="D327" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4">
       <c r="A328" t="s">
         <v>325</v>
       </c>
@@ -5255,8 +5978,11 @@
       <c r="C328" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="329" spans="1:3">
+      <c r="D328" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4">
       <c r="A329" t="s">
         <v>326</v>
       </c>
@@ -5266,24 +5992,27 @@
       <c r="C329" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="331" spans="1:3">
+      <c r="D329" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4">
       <c r="A331" s="1" t="s">
         <v>327</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Complete">
+  <conditionalFormatting sqref="B1:D1048576 E16">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Not started">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not started">
       <formula>NOT(ISERROR(SEARCH("Not started",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Not porting">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Not porting">
       <formula>NOT(ISERROR(SEARCH("Not porting",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finish Rectangle, swift tweaks
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="0" windowWidth="20260" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="341">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1654,11 +1654,8 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>192</v>
-      </c>
-      <c r="C16" t="s">
-        <v>328</v>
       </c>
       <c r="D16" t="s">
         <v>191</v>
@@ -2074,11 +2071,8 @@
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>192</v>
-      </c>
-      <c r="C46" t="s">
-        <v>328</v>
       </c>
       <c r="D46" t="s">
         <v>191</v>
@@ -2522,11 +2516,8 @@
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B78" t="s">
-        <v>191</v>
-      </c>
       <c r="C78" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D78" t="s">
         <v>191</v>
@@ -3071,11 +3062,8 @@
       <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>192</v>
-      </c>
-      <c r="C117" t="s">
-        <v>191</v>
       </c>
       <c r="D117" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Swift doesn't need defaultvalue code, didSet: not called by init
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="341">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1598,11 +1598,8 @@
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>328</v>
-      </c>
       <c r="C12" t="s">
-        <v>328</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
         <v>191</v>
@@ -1644,7 +1641,7 @@
         <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D15" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
BoundingRectangle complete, few other type fixes, start TerrainProvider
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="380" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="341">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2247,11 +2247,8 @@
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>192</v>
-      </c>
-      <c r="C59" t="s">
-        <v>191</v>
       </c>
       <c r="D59" t="s">
         <v>191</v>
@@ -3532,11 +3529,8 @@
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
         <v>192</v>
-      </c>
-      <c r="C151" t="s">
-        <v>191</v>
       </c>
       <c r="D151" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Implement Cartesian4.swift, update other cartesians
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="380" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="5520" yWindow="300" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="340">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1033,9 +1033,6 @@
   </si>
   <si>
     <t>Swift port</t>
-  </si>
-  <si>
-    <t>Missing array return bug</t>
   </si>
   <si>
     <t>Tests</t>
@@ -1486,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1513,7 +1510,7 @@
         <v>337</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -1584,11 +1581,8 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>192</v>
-      </c>
-      <c r="C11" t="s">
-        <v>191</v>
       </c>
       <c r="D11" t="s">
         <v>191</v>
@@ -1637,11 +1631,8 @@
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>192</v>
-      </c>
-      <c r="C15" t="s">
-        <v>328</v>
       </c>
       <c r="D15" t="s">
         <v>191</v>
@@ -1658,7 +1649,7 @@
         <v>191</v>
       </c>
       <c r="E16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1900,11 +1891,8 @@
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>191</v>
-      </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D34" t="s">
         <v>191</v>
@@ -2103,7 +2091,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -2117,7 +2105,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -2131,7 +2119,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -2145,21 +2133,18 @@
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>328</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
         <v>191</v>
       </c>
-      <c r="E52" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -2173,7 +2158,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -2187,7 +2172,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2201,7 +2186,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -2215,7 +2200,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2229,7 +2214,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -2243,7 +2228,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -2254,7 +2239,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2253,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -2282,7 +2267,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
@@ -2296,7 +2281,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
@@ -2310,7 +2295,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -3277,11 +3262,8 @@
       <c r="A133" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>192</v>
-      </c>
-      <c r="C133" t="s">
-        <v>191</v>
       </c>
       <c r="D133" t="s">
         <v>191</v>
@@ -3291,11 +3273,8 @@
       <c r="A134" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>192</v>
-      </c>
-      <c r="C134" t="s">
-        <v>191</v>
       </c>
       <c r="D134" t="s">
         <v>191</v>
@@ -3305,11 +3284,8 @@
       <c r="A135" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>192</v>
-      </c>
-      <c r="C135" t="s">
-        <v>191</v>
       </c>
       <c r="D135" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Remove old Obj-C types, fix Geometry
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="300" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="20380" yWindow="2440" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="341">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1099,121 +1099,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1600,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2374,11 +2260,8 @@
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
-        <v>191</v>
-      </c>
       <c r="C61" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D61" t="s">
         <v>191</v>
@@ -2388,11 +2271,8 @@
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
-        <v>191</v>
-      </c>
       <c r="C62" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D62" t="s">
         <v>191</v>
@@ -2402,11 +2282,8 @@
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>191</v>
-      </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
         <v>191</v>
@@ -6069,16 +5946,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:D1048576 E16:E18">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Not started">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not started">
       <formula>NOT(ISERROR(SEARCH("Not started",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Not porting">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Not porting">
       <formula>NOT(ISERROR(SEARCH("Not porting",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add PixelFormat, start implementing renderer texture
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="2440" windowWidth="27200" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="2160" yWindow="0" windowWidth="28060" windowHeight="17700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="342">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1042,6 +1042,9 @@
   </si>
   <si>
     <t>" "</t>
+  </si>
+  <si>
+    <t>Needs function array</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2679,11 +2682,8 @@
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>328</v>
-      </c>
-      <c r="C92" t="s">
-        <v>191</v>
       </c>
       <c r="D92" t="s">
         <v>191</v>
@@ -4120,11 +4120,8 @@
       <c r="A198" t="s">
         <v>197</v>
       </c>
-      <c r="B198" t="s">
-        <v>191</v>
-      </c>
       <c r="C198" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D198" t="s">
         <v>191</v>
@@ -4134,11 +4131,8 @@
       <c r="A199" t="s">
         <v>198</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>328</v>
-      </c>
-      <c r="C199" t="s">
-        <v>191</v>
       </c>
       <c r="D199" t="s">
         <v>191</v>
@@ -4148,11 +4142,8 @@
       <c r="A200" t="s">
         <v>199</v>
       </c>
-      <c r="B200" t="s">
-        <v>191</v>
-      </c>
       <c r="C200" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D200" t="s">
         <v>191</v>
@@ -4176,11 +4167,8 @@
       <c r="A202" t="s">
         <v>201</v>
       </c>
-      <c r="B202" t="s">
-        <v>328</v>
-      </c>
       <c r="C202" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D202" t="s">
         <v>191</v>
@@ -4193,11 +4181,8 @@
       <c r="A203" t="s">
         <v>202</v>
       </c>
-      <c r="B203" t="s">
-        <v>191</v>
-      </c>
       <c r="C203" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D203" t="s">
         <v>191</v>
@@ -4221,11 +4206,8 @@
       <c r="A205" t="s">
         <v>204</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>328</v>
-      </c>
-      <c r="C205" t="s">
-        <v>191</v>
       </c>
       <c r="D205" t="s">
         <v>191</v>
@@ -4266,17 +4248,14 @@
       <c r="A208" t="s">
         <v>207</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>328</v>
       </c>
-      <c r="C208" t="s">
-        <v>191</v>
-      </c>
       <c r="D208" t="s">
         <v>191</v>
       </c>
       <c r="E208" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4325,11 +4304,8 @@
       <c r="A212" t="s">
         <v>211</v>
       </c>
-      <c r="B212" t="s">
-        <v>191</v>
-      </c>
       <c r="C212" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D212" t="s">
         <v>191</v>
@@ -4339,11 +4315,8 @@
       <c r="A213" t="s">
         <v>212</v>
       </c>
-      <c r="B213" t="s">
-        <v>191</v>
-      </c>
       <c r="C213" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D213" t="s">
         <v>191</v>
@@ -4353,11 +4326,8 @@
       <c r="A214" t="s">
         <v>213</v>
       </c>
-      <c r="B214" t="s">
-        <v>191</v>
-      </c>
       <c r="C214" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D214" t="s">
         <v>191</v>
@@ -4409,11 +4379,8 @@
       <c r="A218" t="s">
         <v>217</v>
       </c>
-      <c r="B218" t="s">
-        <v>191</v>
-      </c>
       <c r="C218" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D218" t="s">
         <v>191</v>
@@ -4426,11 +4393,8 @@
       <c r="A219" t="s">
         <v>218</v>
       </c>
-      <c r="B219" t="s">
-        <v>191</v>
-      </c>
       <c r="C219" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D219" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Basic CesiumKit root class, implement more Scene types
</commit_message>
<xml_diff>
--- a/CesiumStatus.xlsx
+++ b/CesiumStatus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="342">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -1489,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B236" sqref="B236"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5396,11 +5396,8 @@
       <c r="A295" t="s">
         <v>292</v>
       </c>
-      <c r="B295" t="s">
-        <v>191</v>
-      </c>
       <c r="C295" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="D295" t="s">
         <v>191</v>
@@ -5466,11 +5463,8 @@
       <c r="A300" t="s">
         <v>297</v>
       </c>
-      <c r="B300" t="s">
+      <c r="C300" t="s">
         <v>328</v>
-      </c>
-      <c r="C300" t="s">
-        <v>191</v>
       </c>
       <c r="D300" t="s">
         <v>191</v>

</xml_diff>